<commit_message>
excel support for multiple companies
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -11,30 +11,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Google</t>
   </si>
   <si>
-    <t>https://www.google.com/url?q=https://www.linkedin.com/in/robertprescott&amp;sa=U&amp;ved=2ahUKEwjerNrbhMDwAhUSXKwKHXE1DbsQFjACegQICRAB&amp;usg=AOvVaw1IqUCHN0_8kxWYA7xM9Wcq</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?q=https://www.linkedin.com/in/fernandoterrero&amp;sa=U&amp;ved=2ahUKEwjerNrbhMDwAhUSXKwKHXE1DbsQFjADegQICBAB&amp;usg=AOvVaw0axfhTW7l1LJ2W2i6Hibrw</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?q=https://www.linkedin.com/in/petersenjordan&amp;sa=U&amp;ved=2ahUKEwjerNrbhMDwAhUSXKwKHXE1DbsQFjAEegQIBxAB&amp;usg=AOvVaw3BOZlbr8gAnnZC1DbOu6NR</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?q=https://www.linkedin.com/in/jacq-morrill-12a41983&amp;sa=U&amp;ved=2ahUKEwjerNrbhMDwAhUSXKwKHXE1DbsQFjAGegQIARAB&amp;usg=AOvVaw3yI1Js1rkRDcVwqkLQhD1j</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?q=https://www.linkedin.com/in/chantal-penton-1165b461&amp;sa=U&amp;ved=2ahUKEwjerNrbhMDwAhUSXKwKHXE1DbsQFjAHegQIABAB&amp;usg=AOvVaw2zeXbunTFaR-tDen-MvT8k</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?q=https://www.linkedin.com/in/latasha-smith-73996b4b&amp;sa=U&amp;ved=2ahUKEwjerNrbhMDwAhUSXKwKHXE1DbsQFjAIegQIAxAB&amp;usg=AOvVaw0D52hJJ7UKjXLkx7t38qL3</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?q=https://www.linkedin.com/in/ericbarradas&amp;sa=U&amp;ved=2ahUKEwjerNrbhMDwAhUSXKwKHXE1DbsQFjAJegQIBBAB&amp;usg=AOvVaw0gNgHxxHBaoa5ZuLisE081</t>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/robertprescott&amp;sa=U&amp;ved=2ahUKEwinppSc0cHwAhWDup4KHVatAA8QFjACegQICBAB&amp;usg=AOvVaw2FkHodd__nRdVJRuAO1jr5</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/kyleroysmith&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjAAegQIBRAB&amp;usg=AOvVaw2emxTBlugLKjqgZAd6mefv</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/fernandoterrero&amp;sa=U&amp;ved=2ahUKEwinppSc0cHwAhWDup4KHVatAA8QFjADegQIBxAB&amp;usg=AOvVaw3AhEzheb6pqW58ETymWM_t</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/amymil&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjABegQICRAB&amp;usg=AOvVaw1MYjGwuziqtwzdpWlgz7v6</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/petersenjordan&amp;sa=U&amp;ved=2ahUKEwinppSc0cHwAhWDup4KHVatAA8QFjAEegQICRAB&amp;usg=AOvVaw2zkQOovCLCquzUxvZngMz2</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/tripti-vishwakarma&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjACegQIBxAB&amp;usg=AOvVaw1Kv2GnYCmAR_vCbYRfQb9h</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/jacq-morrill-12a41983&amp;sa=U&amp;ved=2ahUKEwinppSc0cHwAhWDup4KHVatAA8QFjAFegQIABAB&amp;usg=AOvVaw0pFErZl4HLXuQiNz3yYwxW</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/emucken&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjADegQICBAB&amp;usg=AOvVaw1BKb4_hUDIufiwCZwKXlFn</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/ericbarradas&amp;sa=U&amp;ved=2ahUKEwinppSc0cHwAhWDup4KHVatAA8QFjAHegQIAxAB&amp;usg=AOvVaw0pBdsFtdBrCX5EcgkEg2sf</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/jennifer-kemp-71057251&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjAEegQIChAB&amp;usg=AOvVaw1dwP37JjfUA5rKm8MJI8Eq</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/latasha-smith-73996b4b&amp;sa=U&amp;ved=2ahUKEwinppSc0cHwAhWDup4KHVatAA8QFjAIegQIARAB&amp;usg=AOvVaw0yhKNcntbMO2K1Tb3URlNz</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/saramorgan89&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjAFegQIAxAB&amp;usg=AOvVaw0tiQke8z8I1Yc34lzfBPqc</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/chantal-penton-1165b461&amp;sa=U&amp;ved=2ahUKEwinppSc0cHwAhWDup4KHVatAA8QFjAJegQIBRAB&amp;usg=AOvVaw08Dgm_S3q7ZVhBOAx2ixfH</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/danadworman&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjAGegQIAhAB&amp;usg=AOvVaw3JFQGyxV-_XFMaFeVRl1fG</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/claireoc&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjAHegQIBBAB&amp;usg=AOvVaw1aqLKDBcmS6Jp2qkDSOmMr</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https://www.linkedin.com/in/joshmayaws&amp;sa=U&amp;ved=2ahUKEwiHk4at0cHwAhVPrJ4KHRc2C3wQFjAJegQIABAB&amp;usg=AOvVaw3AWcFhLaTzgYMXkj1nms59</t>
   </si>
 </sst>
 </file>
@@ -411,50 +441,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="200" customWidth="1"/>
+    <col min="1" max="2" width="200" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>